<commit_message>
performance enhancements, fix for block size error, tests with Middlebury sequences
</commit_message>
<xml_diff>
--- a/block_sizes.xlsx
+++ b/block_sizes.xlsx
@@ -347,7 +347,7 @@
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -426,7 +426,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>B2/B5</f>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <f>C2/C5</f>
@@ -452,7 +452,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>B3/B5</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C9">
         <f>C3/C5</f>

</xml_diff>

<commit_message>
Performance Improvements, Spiral Search, Multithreaded Block Matching
</commit_message>
<xml_diff>
--- a/block_sizes.xlsx
+++ b/block_sizes.xlsx
@@ -344,25 +344,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U12"/>
+  <dimension ref="A2:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>1280</v>
+        <v>1792</v>
       </c>
       <c r="C2">
         <f>B2/2</f>
-        <v>640</v>
+        <v>896</v>
       </c>
       <c r="D2">
         <f>C2/2</f>
-        <v>320</v>
+        <v>448</v>
+      </c>
+      <c r="E2">
+        <f>D2/2</f>
+        <v>224</v>
       </c>
       <c r="G2">
         <v>512</v>
@@ -397,15 +401,19 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>1920</v>
+        <v>2560</v>
       </c>
       <c r="C3">
         <f>B3/2</f>
-        <v>960</v>
+        <v>1280</v>
       </c>
       <c r="D3">
         <f>C3/2</f>
-        <v>480</v>
+        <v>640</v>
+      </c>
+      <c r="E3">
+        <f>D3/2</f>
+        <v>320</v>
       </c>
       <c r="G3">
         <v>512</v>
@@ -445,6 +453,9 @@
         <v>32</v>
       </c>
       <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
         <v>32</v>
       </c>
       <c r="G5">
@@ -483,15 +494,19 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>B2/B5</f>
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <f>C2/C5</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <f>D2/D5</f>
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <f>E2/E5</f>
+        <v>7</v>
       </c>
       <c r="G8">
         <f>G3/G5</f>
@@ -521,15 +536,19 @@
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>B3/B5</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <f>C3/C5</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <f>D3/D5</f>
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f>E3/E5</f>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -544,6 +563,50 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>584</v>
+      </c>
+      <c r="C18">
+        <f>B18*4</f>
+        <v>2336</v>
+      </c>
+      <c r="E18">
+        <f>B3-C18</f>
+        <v>224</v>
+      </c>
+      <c r="F18">
+        <f>E18/2</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>388</v>
+      </c>
+      <c r="C19">
+        <f>B19*4</f>
+        <v>1552</v>
+      </c>
+      <c r="E19">
+        <f>B2-C19</f>
+        <v>240</v>
+      </c>
+      <c r="F19">
+        <f>E19/2</f>
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>